<commit_message>
Fix aim vs generator all
</commit_message>
<xml_diff>
--- a/TA bab 1-4/Tabel aim vs generator.xlsx
+++ b/TA bab 1-4/Tabel aim vs generator.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="25">
   <si>
     <t>My Bot 3</t>
   </si>
@@ -417,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:O267"/>
+  <dimension ref="B1:M267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
-      <selection activeCell="B205" sqref="B205"/>
+    <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
+      <selection activeCell="B205" sqref="B205:M205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7560,7 +7560,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="193" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B193">
         <v>488798</v>
       </c>
@@ -7598,7 +7598,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="194" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B194">
         <v>488799</v>
       </c>
@@ -7636,7 +7636,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="195" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B195">
         <v>488800</v>
       </c>
@@ -7674,7 +7674,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="196" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B196">
         <v>488801</v>
       </c>
@@ -7712,7 +7712,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="197" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B197">
         <v>488802</v>
       </c>
@@ -7750,7 +7750,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="198" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B198">
         <v>488803</v>
       </c>
@@ -7788,7 +7788,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="199" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B199">
         <v>488804</v>
       </c>
@@ -7826,7 +7826,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="200" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B200">
         <v>488805</v>
       </c>
@@ -7864,12 +7864,50 @@
         <v>100</v>
       </c>
     </row>
-    <row r="205" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B204" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="205" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B205" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="206" spans="2:15" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="C205" t="s">
+        <v>5</v>
+      </c>
+      <c r="D205" t="s">
+        <v>6</v>
+      </c>
+      <c r="E205" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F205" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G205" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H205" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I205" t="s">
+        <v>11</v>
+      </c>
+      <c r="J205" t="s">
+        <v>10</v>
+      </c>
+      <c r="K205" t="s">
+        <v>9</v>
+      </c>
+      <c r="L205" t="s">
+        <v>14</v>
+      </c>
+      <c r="M205" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="206" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B206">
         <v>1</v>
       </c>
@@ -7880,40 +7918,34 @@
         <v>6</v>
       </c>
       <c r="E206" s="1">
-        <v>200</v>
+        <v>2924.68</v>
       </c>
       <c r="F206" s="1">
-        <v>2924.68</v>
-      </c>
-      <c r="G206" s="1">
         <v>539.76</v>
       </c>
-      <c r="H206" s="1" t="s">
-        <v>3</v>
+      <c r="G206">
+        <v>2705.16</v>
+      </c>
+      <c r="H206">
+        <v>530.91</v>
       </c>
       <c r="I206">
+        <v>24</v>
+      </c>
+      <c r="J206">
+        <v>1</v>
+      </c>
+      <c r="K206" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L206">
         <v>160.54</v>
       </c>
-      <c r="J206">
-        <v>1</v>
-      </c>
-      <c r="K206">
-        <v>0</v>
-      </c>
-      <c r="L206">
-        <v>2705.16</v>
-      </c>
       <c r="M206">
-        <v>530.91</v>
-      </c>
-      <c r="N206">
-        <v>24</v>
-      </c>
-      <c r="O206">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="207" spans="2:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B207">
         <v>2</v>
       </c>
@@ -7924,40 +7956,34 @@
         <v>6</v>
       </c>
       <c r="E207" s="1">
-        <v>200</v>
+        <v>2924.68</v>
       </c>
       <c r="F207" s="1">
-        <v>2924.68</v>
-      </c>
-      <c r="G207" s="1">
         <v>539.76</v>
       </c>
-      <c r="H207" s="1" t="s">
-        <v>3</v>
+      <c r="G207">
+        <v>2708.56</v>
+      </c>
+      <c r="H207">
+        <v>525.91</v>
       </c>
       <c r="I207">
+        <v>24</v>
+      </c>
+      <c r="J207">
+        <v>1</v>
+      </c>
+      <c r="K207" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L207">
         <v>161.79</v>
       </c>
-      <c r="J207">
-        <v>1</v>
-      </c>
-      <c r="K207">
-        <v>0</v>
-      </c>
-      <c r="L207">
-        <v>2708.56</v>
-      </c>
       <c r="M207">
-        <v>525.91</v>
-      </c>
-      <c r="N207">
-        <v>24</v>
-      </c>
-      <c r="O207">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="208" spans="2:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B208">
         <v>3</v>
       </c>
@@ -7968,40 +7994,34 @@
         <v>6</v>
       </c>
       <c r="E208" s="1">
-        <v>200</v>
+        <v>2924.68</v>
       </c>
       <c r="F208" s="1">
-        <v>2924.68</v>
-      </c>
-      <c r="G208" s="1">
         <v>539.76</v>
       </c>
-      <c r="H208" s="1" t="s">
-        <v>3</v>
+      <c r="G208">
+        <v>2712.55</v>
+      </c>
+      <c r="H208">
+        <v>521.51</v>
       </c>
       <c r="I208">
+        <v>24</v>
+      </c>
+      <c r="J208">
+        <v>1</v>
+      </c>
+      <c r="K208" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L208">
         <v>162.02000000000001</v>
       </c>
-      <c r="J208">
-        <v>1</v>
-      </c>
-      <c r="K208">
-        <v>0</v>
-      </c>
-      <c r="L208">
-        <v>2712.55</v>
-      </c>
       <c r="M208">
-        <v>521.51</v>
-      </c>
-      <c r="N208">
-        <v>24</v>
-      </c>
-      <c r="O208">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="209" spans="2:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B209">
         <v>4</v>
       </c>
@@ -8012,40 +8032,34 @@
         <v>6</v>
       </c>
       <c r="E209" s="1">
-        <v>200</v>
+        <v>2924.68</v>
       </c>
       <c r="F209" s="1">
-        <v>2924.68</v>
-      </c>
-      <c r="G209" s="1">
         <v>539.76</v>
       </c>
-      <c r="H209" s="1" t="s">
-        <v>3</v>
+      <c r="G209">
+        <v>2717.05</v>
+      </c>
+      <c r="H209">
+        <v>517.71</v>
       </c>
       <c r="I209">
+        <v>24</v>
+      </c>
+      <c r="J209">
+        <v>1</v>
+      </c>
+      <c r="K209" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L209">
         <v>162.22999999999999</v>
       </c>
-      <c r="J209">
-        <v>1</v>
-      </c>
-      <c r="K209">
-        <v>0</v>
-      </c>
-      <c r="L209">
-        <v>2717.05</v>
-      </c>
       <c r="M209">
-        <v>517.71</v>
-      </c>
-      <c r="N209">
-        <v>24</v>
-      </c>
-      <c r="O209">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="210" spans="2:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B210">
         <v>5</v>
       </c>
@@ -8056,40 +8070,34 @@
         <v>6</v>
       </c>
       <c r="E210" s="1">
-        <v>200</v>
+        <v>2924.68</v>
       </c>
       <c r="F210" s="1">
-        <v>2924.68</v>
-      </c>
-      <c r="G210" s="1">
         <v>539.76</v>
       </c>
-      <c r="H210" s="1" t="s">
-        <v>3</v>
+      <c r="G210">
+        <v>2722</v>
+      </c>
+      <c r="H210">
+        <v>514.51</v>
       </c>
       <c r="I210">
+        <v>24</v>
+      </c>
+      <c r="J210">
+        <v>1</v>
+      </c>
+      <c r="K210" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L210">
         <v>162.41</v>
       </c>
-      <c r="J210">
-        <v>1</v>
-      </c>
-      <c r="K210">
-        <v>0</v>
-      </c>
-      <c r="L210">
-        <v>2722</v>
-      </c>
       <c r="M210">
-        <v>514.51</v>
-      </c>
-      <c r="N210">
-        <v>24</v>
-      </c>
-      <c r="O210">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="211" spans="2:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B211">
         <v>6</v>
       </c>
@@ -8100,40 +8108,34 @@
         <v>6</v>
       </c>
       <c r="E211" s="1">
-        <v>200</v>
+        <v>2924.68</v>
       </c>
       <c r="F211" s="1">
-        <v>2924.68</v>
-      </c>
-      <c r="G211" s="1">
         <v>539.76</v>
       </c>
-      <c r="H211" s="1" t="s">
-        <v>3</v>
+      <c r="G211">
+        <v>2727.34</v>
+      </c>
+      <c r="H211">
+        <v>511.91</v>
       </c>
       <c r="I211">
+        <v>24</v>
+      </c>
+      <c r="J211">
+        <v>1</v>
+      </c>
+      <c r="K211" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L211">
         <v>164.11</v>
       </c>
-      <c r="J211">
-        <v>1</v>
-      </c>
-      <c r="K211">
-        <v>0</v>
-      </c>
-      <c r="L211">
-        <v>2727.34</v>
-      </c>
       <c r="M211">
-        <v>511.91</v>
-      </c>
-      <c r="N211">
-        <v>24</v>
-      </c>
-      <c r="O211">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="212" spans="2:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B212">
         <v>7</v>
       </c>
@@ -8144,40 +8146,34 @@
         <v>6</v>
       </c>
       <c r="E212" s="1">
-        <v>200</v>
+        <v>2924.68</v>
       </c>
       <c r="F212" s="1">
-        <v>2924.68</v>
-      </c>
-      <c r="G212" s="1">
         <v>539.76</v>
       </c>
-      <c r="H212" s="1" t="s">
-        <v>3</v>
+      <c r="G212">
+        <v>2733.02</v>
+      </c>
+      <c r="H212">
+        <v>509.91</v>
       </c>
       <c r="I212">
+        <v>24</v>
+      </c>
+      <c r="J212">
+        <v>1</v>
+      </c>
+      <c r="K212" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L212">
         <v>164.33</v>
       </c>
-      <c r="J212">
-        <v>1</v>
-      </c>
-      <c r="K212">
-        <v>0</v>
-      </c>
-      <c r="L212">
-        <v>2733.02</v>
-      </c>
       <c r="M212">
-        <v>509.91</v>
-      </c>
-      <c r="N212">
-        <v>24</v>
-      </c>
-      <c r="O212">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="213" spans="2:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B213">
         <v>8</v>
       </c>
@@ -8188,40 +8184,34 @@
         <v>6</v>
       </c>
       <c r="E213" s="1">
-        <v>200</v>
+        <v>2924.68</v>
       </c>
       <c r="F213" s="1">
-        <v>2924.68</v>
-      </c>
-      <c r="G213" s="1">
         <v>539.76</v>
       </c>
-      <c r="H213" s="1" t="s">
-        <v>1</v>
+      <c r="G213">
+        <v>2738.99</v>
+      </c>
+      <c r="H213">
+        <v>508.51</v>
       </c>
       <c r="I213">
+        <v>24</v>
+      </c>
+      <c r="J213">
+        <v>1</v>
+      </c>
+      <c r="K213" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L213">
         <v>166.54</v>
       </c>
-      <c r="J213">
-        <v>1</v>
-      </c>
-      <c r="K213">
-        <v>0</v>
-      </c>
-      <c r="L213">
-        <v>2738.99</v>
-      </c>
       <c r="M213">
-        <v>508.51</v>
-      </c>
-      <c r="N213">
-        <v>24</v>
-      </c>
-      <c r="O213">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="214" spans="2:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B214">
         <v>9</v>
       </c>
@@ -8232,40 +8222,34 @@
         <v>6</v>
       </c>
       <c r="E214" s="1">
-        <v>200</v>
+        <v>2924.68</v>
       </c>
       <c r="F214" s="1">
-        <v>2924.68</v>
-      </c>
-      <c r="G214" s="1">
         <v>539.76</v>
       </c>
-      <c r="H214" s="1" t="s">
-        <v>3</v>
+      <c r="G214">
+        <v>2745.22</v>
+      </c>
+      <c r="H214">
+        <v>507.71</v>
       </c>
       <c r="I214">
+        <v>24</v>
+      </c>
+      <c r="J214">
+        <v>1</v>
+      </c>
+      <c r="K214" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L214">
         <v>166.85</v>
       </c>
-      <c r="J214">
-        <v>1</v>
-      </c>
-      <c r="K214">
-        <v>0</v>
-      </c>
-      <c r="L214">
-        <v>2745.22</v>
-      </c>
       <c r="M214">
-        <v>507.71</v>
-      </c>
-      <c r="N214">
-        <v>24</v>
-      </c>
-      <c r="O214">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="215" spans="2:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B215">
         <v>10</v>
       </c>
@@ -8276,40 +8260,34 @@
         <v>6</v>
       </c>
       <c r="E215" s="1">
-        <v>200</v>
+        <v>2924.68</v>
       </c>
       <c r="F215" s="1">
-        <v>2924.68</v>
-      </c>
-      <c r="G215" s="1">
         <v>539.76</v>
       </c>
-      <c r="H215" s="1" t="s">
+      <c r="G215">
+        <v>2751.67</v>
+      </c>
+      <c r="H215">
+        <v>507.51</v>
+      </c>
+      <c r="I215">
+        <v>24</v>
+      </c>
+      <c r="J215">
+        <v>1</v>
+      </c>
+      <c r="K215" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I215">
+      <c r="L215">
         <v>167.16</v>
       </c>
-      <c r="J215">
-        <v>1</v>
-      </c>
-      <c r="K215">
-        <v>0</v>
-      </c>
-      <c r="L215">
-        <v>2751.67</v>
-      </c>
       <c r="M215">
-        <v>507.51</v>
-      </c>
-      <c r="N215">
-        <v>24</v>
-      </c>
-      <c r="O215">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="216" spans="2:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B216">
         <v>11</v>
       </c>
@@ -8320,40 +8298,34 @@
         <v>6</v>
       </c>
       <c r="E216" s="1">
-        <v>200</v>
+        <v>2924.68</v>
       </c>
       <c r="F216" s="1">
-        <v>2924.68</v>
-      </c>
-      <c r="G216" s="1">
         <v>531.76</v>
       </c>
-      <c r="H216" s="1" t="s">
-        <v>3</v>
+      <c r="G216">
+        <v>2758.32</v>
+      </c>
+      <c r="H216">
+        <v>507.91</v>
       </c>
       <c r="I216">
+        <v>24</v>
+      </c>
+      <c r="J216">
+        <v>1</v>
+      </c>
+      <c r="K216" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L216">
         <v>171.24</v>
       </c>
-      <c r="J216">
-        <v>1</v>
-      </c>
-      <c r="K216">
-        <v>0</v>
-      </c>
-      <c r="L216">
-        <v>2758.32</v>
-      </c>
       <c r="M216">
-        <v>507.91</v>
-      </c>
-      <c r="N216">
-        <v>24</v>
-      </c>
-      <c r="O216">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="217" spans="2:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B217">
         <v>12</v>
       </c>
@@ -8364,40 +8336,34 @@
         <v>6</v>
       </c>
       <c r="E217" s="1">
-        <v>200</v>
+        <v>2924.68</v>
       </c>
       <c r="F217" s="1">
-        <v>2924.68</v>
-      </c>
-      <c r="G217" s="1">
         <v>524.36</v>
       </c>
-      <c r="H217" s="1" t="s">
-        <v>3</v>
+      <c r="G217">
+        <v>2764.82</v>
+      </c>
+      <c r="H217">
+        <v>508.84</v>
       </c>
       <c r="I217">
+        <v>24</v>
+      </c>
+      <c r="J217">
+        <v>1</v>
+      </c>
+      <c r="K217" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L217">
         <v>175.8</v>
       </c>
-      <c r="J217">
-        <v>1</v>
-      </c>
-      <c r="K217">
-        <v>0</v>
-      </c>
-      <c r="L217">
-        <v>2764.82</v>
-      </c>
       <c r="M217">
-        <v>508.84</v>
-      </c>
-      <c r="N217">
-        <v>24</v>
-      </c>
-      <c r="O217">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="218" spans="2:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B218">
         <v>13</v>
       </c>
@@ -8408,40 +8374,34 @@
         <v>6</v>
       </c>
       <c r="E218" s="1">
-        <v>200</v>
+        <v>2924.68</v>
       </c>
       <c r="F218" s="1">
-        <v>2924.68</v>
-      </c>
-      <c r="G218" s="1">
         <v>511.36</v>
       </c>
-      <c r="H218" s="1" t="s">
-        <v>3</v>
+      <c r="G218">
+        <v>2778.05</v>
+      </c>
+      <c r="H218">
+        <v>512.41999999999996</v>
       </c>
       <c r="I218">
+        <v>112</v>
+      </c>
+      <c r="J218">
+        <v>1</v>
+      </c>
+      <c r="K218" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L218">
         <v>184.8</v>
       </c>
-      <c r="J218">
-        <v>1</v>
-      </c>
-      <c r="K218">
-        <v>0</v>
-      </c>
-      <c r="L218">
-        <v>2778.05</v>
-      </c>
       <c r="M218">
-        <v>512.41999999999996</v>
-      </c>
-      <c r="N218">
-        <v>112</v>
-      </c>
-      <c r="O218">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="219" spans="2:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B219">
         <v>14</v>
       </c>
@@ -8452,40 +8412,34 @@
         <v>6</v>
       </c>
       <c r="E219" s="1">
-        <v>200</v>
+        <v>2924.68</v>
       </c>
       <c r="F219" s="1">
-        <v>2924.68</v>
-      </c>
-      <c r="G219" s="1">
         <v>505.76</v>
       </c>
-      <c r="H219" s="1" t="s">
-        <v>3</v>
+      <c r="G219">
+        <v>2784.78</v>
+      </c>
+      <c r="H219">
+        <v>515.08000000000004</v>
       </c>
       <c r="I219">
+        <v>112</v>
+      </c>
+      <c r="J219">
+        <v>1</v>
+      </c>
+      <c r="K219" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L219">
         <v>189.02</v>
       </c>
-      <c r="J219">
-        <v>1</v>
-      </c>
-      <c r="K219">
-        <v>0</v>
-      </c>
-      <c r="L219">
-        <v>2784.78</v>
-      </c>
       <c r="M219">
-        <v>515.08000000000004</v>
-      </c>
-      <c r="N219">
-        <v>112</v>
-      </c>
-      <c r="O219">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="220" spans="2:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="220" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B220">
         <v>15</v>
       </c>
@@ -8496,40 +8450,34 @@
         <v>6</v>
       </c>
       <c r="E220" s="1">
-        <v>200</v>
+        <v>2924.68</v>
       </c>
       <c r="F220" s="1">
-        <v>2924.68</v>
-      </c>
-      <c r="G220" s="1">
         <v>500.76</v>
       </c>
-      <c r="H220" s="1" t="s">
+      <c r="G220">
+        <v>2791.37</v>
+      </c>
+      <c r="H220">
+        <v>518.24</v>
+      </c>
+      <c r="I220">
+        <v>112</v>
+      </c>
+      <c r="J220">
+        <v>1</v>
+      </c>
+      <c r="K220" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I220">
+      <c r="L220">
         <v>193.17</v>
       </c>
-      <c r="J220">
-        <v>1</v>
-      </c>
-      <c r="K220">
-        <v>0</v>
-      </c>
-      <c r="L220">
-        <v>2791.37</v>
-      </c>
       <c r="M220">
-        <v>518.24</v>
-      </c>
-      <c r="N220">
-        <v>112</v>
-      </c>
-      <c r="O220">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="221" spans="2:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B221">
         <v>16</v>
       </c>
@@ -8540,40 +8488,34 @@
         <v>6</v>
       </c>
       <c r="E221" s="1">
-        <v>200</v>
+        <v>2924.68</v>
       </c>
       <c r="F221" s="1">
-        <v>2924.68</v>
-      </c>
-      <c r="G221" s="1">
         <v>496.36</v>
       </c>
-      <c r="H221" s="1" t="s">
-        <v>1</v>
+      <c r="G221">
+        <v>2797.85</v>
+      </c>
+      <c r="H221">
+        <v>521.91</v>
       </c>
       <c r="I221">
+        <v>112</v>
+      </c>
+      <c r="J221">
+        <v>1</v>
+      </c>
+      <c r="K221" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L221">
         <v>197.18</v>
       </c>
-      <c r="J221">
-        <v>1</v>
-      </c>
-      <c r="K221">
-        <v>0</v>
-      </c>
-      <c r="L221">
-        <v>2797.85</v>
-      </c>
       <c r="M221">
-        <v>521.91</v>
-      </c>
-      <c r="N221">
-        <v>112</v>
-      </c>
-      <c r="O221">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="222" spans="2:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="222" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B222">
         <v>17</v>
       </c>
@@ -8584,40 +8526,34 @@
         <v>6</v>
       </c>
       <c r="E222" s="1">
-        <v>200</v>
+        <v>2924.45</v>
       </c>
       <c r="F222" s="1">
-        <v>2924.45</v>
-      </c>
-      <c r="G222" s="1">
         <v>492.56</v>
       </c>
-      <c r="H222" s="1" t="s">
-        <v>3</v>
+      <c r="G222">
+        <v>2804.19</v>
+      </c>
+      <c r="H222">
+        <v>526.11</v>
       </c>
       <c r="I222">
+        <v>112</v>
+      </c>
+      <c r="J222">
+        <v>1</v>
+      </c>
+      <c r="K222" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L222">
         <v>201.1</v>
       </c>
-      <c r="J222">
-        <v>1</v>
-      </c>
-      <c r="K222">
-        <v>0</v>
-      </c>
-      <c r="L222">
-        <v>2804.19</v>
-      </c>
       <c r="M222">
-        <v>526.11</v>
-      </c>
-      <c r="N222">
-        <v>112</v>
-      </c>
-      <c r="O222">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="223" spans="2:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="223" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B223">
         <v>18</v>
       </c>
@@ -8628,40 +8564,34 @@
         <v>6</v>
       </c>
       <c r="E223" s="1">
-        <v>200</v>
+        <v>2924.45</v>
       </c>
       <c r="F223" s="1">
-        <v>2924.45</v>
-      </c>
-      <c r="G223" s="1">
         <v>489.36</v>
       </c>
-      <c r="H223" s="1" t="s">
-        <v>3</v>
+      <c r="G223">
+        <v>2810.51</v>
+      </c>
+      <c r="H223">
+        <v>528.01</v>
       </c>
       <c r="I223">
+        <v>112</v>
+      </c>
+      <c r="J223">
+        <v>1</v>
+      </c>
+      <c r="K223" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L223">
         <v>203.01</v>
       </c>
-      <c r="J223">
-        <v>1</v>
-      </c>
-      <c r="K223">
-        <v>0</v>
-      </c>
-      <c r="L223">
-        <v>2810.51</v>
-      </c>
       <c r="M223">
-        <v>528.01</v>
-      </c>
-      <c r="N223">
-        <v>112</v>
-      </c>
-      <c r="O223">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="224" spans="2:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="224" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B224">
         <v>19</v>
       </c>
@@ -8672,40 +8602,34 @@
         <v>6</v>
       </c>
       <c r="E224" s="1">
-        <v>200</v>
+        <v>2924.45</v>
       </c>
       <c r="F224" s="1">
-        <v>2924.45</v>
-      </c>
-      <c r="G224" s="1">
         <v>486.76</v>
       </c>
-      <c r="H224" s="1" t="s">
-        <v>3</v>
+      <c r="G224">
+        <v>2816.63</v>
+      </c>
+      <c r="H224">
+        <v>528.01</v>
       </c>
       <c r="I224">
+        <v>112</v>
+      </c>
+      <c r="J224">
+        <v>1</v>
+      </c>
+      <c r="K224" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L224">
         <v>206.71</v>
       </c>
-      <c r="J224">
-        <v>1</v>
-      </c>
-      <c r="K224">
-        <v>0</v>
-      </c>
-      <c r="L224">
-        <v>2816.63</v>
-      </c>
       <c r="M224">
-        <v>528.01</v>
-      </c>
-      <c r="N224">
-        <v>112</v>
-      </c>
-      <c r="O224">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="225" spans="2:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="225" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B225">
         <v>20</v>
       </c>
@@ -8716,40 +8640,34 @@
         <v>6</v>
       </c>
       <c r="E225" s="1">
-        <v>200</v>
+        <v>2924.45</v>
       </c>
       <c r="F225" s="1">
-        <v>2924.45</v>
-      </c>
-      <c r="G225" s="1">
         <v>484.76</v>
       </c>
-      <c r="H225" s="1" t="s">
-        <v>3</v>
+      <c r="G225">
+        <v>2820.91</v>
+      </c>
+      <c r="H225">
+        <v>528.01</v>
       </c>
       <c r="I225">
+        <v>112</v>
+      </c>
+      <c r="J225">
+        <v>1</v>
+      </c>
+      <c r="K225" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L225">
         <v>205.36</v>
       </c>
-      <c r="J225">
-        <v>1</v>
-      </c>
-      <c r="K225">
-        <v>0</v>
-      </c>
-      <c r="L225">
-        <v>2820.91</v>
-      </c>
       <c r="M225">
-        <v>528.01</v>
-      </c>
-      <c r="N225">
-        <v>112</v>
-      </c>
-      <c r="O225">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="226" spans="2:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="226" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B226">
         <v>21</v>
       </c>
@@ -8760,40 +8678,34 @@
         <v>6</v>
       </c>
       <c r="E226" s="1">
-        <v>200</v>
+        <v>2924.45</v>
       </c>
       <c r="F226" s="1">
-        <v>2924.45</v>
-      </c>
-      <c r="G226" s="1">
         <v>483.36</v>
       </c>
-      <c r="H226" s="1" t="s">
+      <c r="G226">
+        <v>2823.29</v>
+      </c>
+      <c r="H226">
+        <v>528.1</v>
+      </c>
+      <c r="I226">
+        <v>112</v>
+      </c>
+      <c r="J226">
+        <v>1</v>
+      </c>
+      <c r="K226" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I226">
+      <c r="L226">
         <v>203.88</v>
       </c>
-      <c r="J226">
-        <v>1</v>
-      </c>
-      <c r="K226">
-        <v>0</v>
-      </c>
-      <c r="L226">
-        <v>2823.29</v>
-      </c>
       <c r="M226">
-        <v>528.1</v>
-      </c>
-      <c r="N226">
-        <v>112</v>
-      </c>
-      <c r="O226">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="227" spans="2:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="227" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B227">
         <v>22</v>
       </c>
@@ -8804,40 +8716,34 @@
         <v>6</v>
       </c>
       <c r="E227" s="1">
-        <v>200</v>
+        <v>2924.45</v>
       </c>
       <c r="F227" s="1">
-        <v>2924.45</v>
-      </c>
-      <c r="G227" s="1">
         <v>482.56</v>
       </c>
-      <c r="H227" s="1" t="s">
-        <v>3</v>
+      <c r="G227">
+        <v>2824.32</v>
+      </c>
+      <c r="H227">
+        <v>528.19000000000005</v>
       </c>
       <c r="I227">
+        <v>112</v>
+      </c>
+      <c r="J227">
+        <v>1</v>
+      </c>
+      <c r="K227" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L227">
         <v>201.02</v>
       </c>
-      <c r="J227">
-        <v>1</v>
-      </c>
-      <c r="K227">
-        <v>0</v>
-      </c>
-      <c r="L227">
-        <v>2824.32</v>
-      </c>
       <c r="M227">
-        <v>528.19000000000005</v>
-      </c>
-      <c r="N227">
-        <v>112</v>
-      </c>
-      <c r="O227">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="228" spans="2:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="228" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B228">
         <v>23</v>
       </c>
@@ -8848,40 +8754,34 @@
         <v>6</v>
       </c>
       <c r="E228" s="1">
-        <v>200</v>
+        <v>2924.45</v>
       </c>
       <c r="F228" s="1">
-        <v>2924.45</v>
-      </c>
-      <c r="G228" s="1">
         <v>482.36</v>
       </c>
-      <c r="H228" s="1" t="s">
-        <v>3</v>
+      <c r="G228">
+        <v>2823.86</v>
+      </c>
+      <c r="H228">
+        <v>528.4</v>
       </c>
       <c r="I228">
+        <v>112</v>
+      </c>
+      <c r="J228">
+        <v>1</v>
+      </c>
+      <c r="K228" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L228">
         <v>198.43</v>
       </c>
-      <c r="J228">
-        <v>1</v>
-      </c>
-      <c r="K228">
-        <v>0</v>
-      </c>
-      <c r="L228">
-        <v>2823.86</v>
-      </c>
       <c r="M228">
-        <v>528.4</v>
-      </c>
-      <c r="N228">
-        <v>112</v>
-      </c>
-      <c r="O228">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="229" spans="2:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="229" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B229">
         <v>24</v>
       </c>
@@ -8892,40 +8792,34 @@
         <v>6</v>
       </c>
       <c r="E229" s="1">
-        <v>200</v>
+        <v>2924.45</v>
       </c>
       <c r="F229" s="1">
-        <v>2924.45</v>
-      </c>
-      <c r="G229" s="1">
         <v>482.76</v>
       </c>
-      <c r="H229" s="1" t="s">
-        <v>3</v>
+      <c r="G229">
+        <v>2822.86</v>
+      </c>
+      <c r="H229">
+        <v>528.4</v>
       </c>
       <c r="I229">
+        <v>112</v>
+      </c>
+      <c r="J229">
+        <v>1</v>
+      </c>
+      <c r="K229" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L229">
         <v>195.4</v>
       </c>
-      <c r="J229">
-        <v>1</v>
-      </c>
-      <c r="K229">
-        <v>0</v>
-      </c>
-      <c r="L229">
-        <v>2822.86</v>
-      </c>
       <c r="M229">
-        <v>528.4</v>
-      </c>
-      <c r="N229">
-        <v>112</v>
-      </c>
-      <c r="O229">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="230" spans="2:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="230" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B230">
         <v>25</v>
       </c>
@@ -8936,40 +8830,34 @@
         <v>6</v>
       </c>
       <c r="E230" s="1">
-        <v>200</v>
+        <v>2924.45</v>
       </c>
       <c r="F230" s="1">
-        <v>2924.45</v>
-      </c>
-      <c r="G230" s="1">
         <v>483.76</v>
       </c>
-      <c r="H230" s="1" t="s">
-        <v>3</v>
+      <c r="G230">
+        <v>2820.58</v>
+      </c>
+      <c r="H230">
+        <v>528.4</v>
       </c>
       <c r="I230">
+        <v>112</v>
+      </c>
+      <c r="J230">
+        <v>1</v>
+      </c>
+      <c r="K230" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L230">
         <v>192.1</v>
       </c>
-      <c r="J230">
-        <v>1</v>
-      </c>
-      <c r="K230">
-        <v>0</v>
-      </c>
-      <c r="L230">
-        <v>2820.58</v>
-      </c>
       <c r="M230">
-        <v>528.4</v>
-      </c>
-      <c r="N230">
-        <v>112</v>
-      </c>
-      <c r="O230">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="231" spans="2:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="231" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B231">
         <v>26</v>
       </c>
@@ -8980,40 +8868,34 @@
         <v>6</v>
       </c>
       <c r="E231" s="1">
-        <v>200</v>
+        <v>2924.45</v>
       </c>
       <c r="F231" s="1">
-        <v>2924.45</v>
-      </c>
-      <c r="G231" s="1">
         <v>485.36</v>
       </c>
-      <c r="H231" s="1" t="s">
-        <v>3</v>
+      <c r="G231">
+        <v>2817.56</v>
+      </c>
+      <c r="H231">
+        <v>528.4</v>
       </c>
       <c r="I231">
+        <v>112</v>
+      </c>
+      <c r="J231">
+        <v>1</v>
+      </c>
+      <c r="K231" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L231">
         <v>188.68</v>
       </c>
-      <c r="J231">
-        <v>1</v>
-      </c>
-      <c r="K231">
-        <v>0</v>
-      </c>
-      <c r="L231">
-        <v>2817.56</v>
-      </c>
       <c r="M231">
-        <v>528.4</v>
-      </c>
-      <c r="N231">
-        <v>112</v>
-      </c>
-      <c r="O231">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="232" spans="2:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="232" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B232">
         <v>27</v>
       </c>
@@ -9024,40 +8906,34 @@
         <v>6</v>
       </c>
       <c r="E232" s="1">
-        <v>200</v>
+        <v>2924.45</v>
       </c>
       <c r="F232" s="1">
-        <v>2924.45</v>
-      </c>
-      <c r="G232" s="1">
         <v>487.56</v>
       </c>
-      <c r="H232" s="1" t="s">
-        <v>3</v>
+      <c r="G232">
+        <v>2813.9</v>
+      </c>
+      <c r="H232">
+        <v>528.4</v>
       </c>
       <c r="I232">
+        <v>112</v>
+      </c>
+      <c r="J232">
+        <v>1</v>
+      </c>
+      <c r="K232" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L232">
         <v>185.2</v>
       </c>
-      <c r="J232">
-        <v>1</v>
-      </c>
-      <c r="K232">
-        <v>0</v>
-      </c>
-      <c r="L232">
-        <v>2813.9</v>
-      </c>
       <c r="M232">
-        <v>528.4</v>
-      </c>
-      <c r="N232">
-        <v>112</v>
-      </c>
-      <c r="O232">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="233" spans="2:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="233" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B233">
         <v>28</v>
       </c>
@@ -9068,40 +8944,34 @@
         <v>6</v>
       </c>
       <c r="E233">
-        <v>200</v>
+        <v>2385.81</v>
       </c>
       <c r="F233">
-        <v>2385.81</v>
+        <v>585.64</v>
       </c>
       <c r="G233">
-        <v>585.64</v>
-      </c>
-      <c r="H233" t="s">
-        <v>1</v>
+        <v>2007.27</v>
+      </c>
+      <c r="H233">
+        <v>612.47</v>
       </c>
       <c r="I233">
+        <v>0</v>
+      </c>
+      <c r="J233">
+        <v>0</v>
+      </c>
+      <c r="K233" t="s">
+        <v>1</v>
+      </c>
+      <c r="L233">
         <v>171.07</v>
       </c>
-      <c r="J233">
-        <v>0</v>
-      </c>
-      <c r="K233">
-        <v>0</v>
-      </c>
-      <c r="L233">
-        <v>2007.27</v>
-      </c>
       <c r="M233">
-        <v>612.47</v>
-      </c>
-      <c r="N233">
-        <v>0</v>
-      </c>
-      <c r="O233">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="234" spans="2:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="234" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B234">
         <v>29</v>
       </c>
@@ -9112,40 +8982,34 @@
         <v>6</v>
       </c>
       <c r="E234">
-        <v>200</v>
+        <v>2381.31</v>
       </c>
       <c r="F234">
-        <v>2381.31</v>
+        <v>588.04</v>
       </c>
       <c r="G234">
-        <v>588.04</v>
-      </c>
-      <c r="H234" t="s">
-        <v>1</v>
+        <v>2011.27</v>
+      </c>
+      <c r="H234">
+        <v>606.47</v>
       </c>
       <c r="I234">
+        <v>0</v>
+      </c>
+      <c r="J234">
+        <v>0</v>
+      </c>
+      <c r="K234" t="s">
+        <v>1</v>
+      </c>
+      <c r="L234">
         <v>167.87</v>
       </c>
-      <c r="J234">
-        <v>0</v>
-      </c>
-      <c r="K234">
-        <v>0</v>
-      </c>
-      <c r="L234">
-        <v>2011.27</v>
-      </c>
       <c r="M234">
-        <v>606.47</v>
-      </c>
-      <c r="N234">
-        <v>0</v>
-      </c>
-      <c r="O234">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="235" spans="2:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="235" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B235">
         <v>30</v>
       </c>
@@ -9156,40 +9020,34 @@
         <v>6</v>
       </c>
       <c r="E235">
-        <v>200</v>
+        <v>2376.81</v>
       </c>
       <c r="F235">
-        <v>2376.81</v>
+        <v>591.04</v>
       </c>
       <c r="G235">
-        <v>591.04</v>
-      </c>
-      <c r="H235" t="s">
+        <v>2013.76</v>
+      </c>
+      <c r="H235">
+        <v>606.47</v>
+      </c>
+      <c r="I235">
+        <v>0</v>
+      </c>
+      <c r="J235">
+        <v>0</v>
+      </c>
+      <c r="K235" t="s">
         <v>2</v>
       </c>
-      <c r="I235">
+      <c r="L235">
         <v>165.44</v>
       </c>
-      <c r="J235">
-        <v>0</v>
-      </c>
-      <c r="K235">
-        <v>0</v>
-      </c>
-      <c r="L235">
-        <v>2013.76</v>
-      </c>
       <c r="M235">
-        <v>606.47</v>
-      </c>
-      <c r="N235">
-        <v>0</v>
-      </c>
-      <c r="O235">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="236" spans="2:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="236" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B236" t="s">
         <v>17</v>
       </c>
@@ -9205,10 +9063,10 @@
       <c r="F236" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G236" s="1" t="s">
+      <c r="G236" t="s">
         <v>17</v>
       </c>
-      <c r="H236" s="1" t="s">
+      <c r="H236" t="s">
         <v>17</v>
       </c>
       <c r="I236" t="s">
@@ -9217,7 +9075,7 @@
       <c r="J236" t="s">
         <v>17</v>
       </c>
-      <c r="K236" t="s">
+      <c r="K236" s="1" t="s">
         <v>17</v>
       </c>
       <c r="L236" t="s">
@@ -9226,14 +9084,8 @@
       <c r="M236" t="s">
         <v>17</v>
       </c>
-      <c r="N236" t="s">
-        <v>17</v>
-      </c>
-      <c r="O236" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="237" spans="2:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="237" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B237" t="s">
         <v>17</v>
       </c>
@@ -9249,10 +9101,10 @@
       <c r="F237" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G237" s="1" t="s">
+      <c r="G237" t="s">
         <v>17</v>
       </c>
-      <c r="H237" s="1" t="s">
+      <c r="H237" t="s">
         <v>17</v>
       </c>
       <c r="I237" t="s">
@@ -9261,7 +9113,7 @@
       <c r="J237" t="s">
         <v>17</v>
       </c>
-      <c r="K237" t="s">
+      <c r="K237" s="1" t="s">
         <v>17</v>
       </c>
       <c r="L237" t="s">
@@ -9270,14 +9122,8 @@
       <c r="M237" t="s">
         <v>17</v>
       </c>
-      <c r="N237" t="s">
-        <v>17</v>
-      </c>
-      <c r="O237" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="238" spans="2:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="238" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B238">
         <v>3144436</v>
       </c>
@@ -9287,41 +9133,35 @@
       <c r="D238">
         <v>0</v>
       </c>
-      <c r="E238">
-        <v>100</v>
+      <c r="E238" s="1">
+        <v>1863.37</v>
       </c>
       <c r="F238" s="1">
-        <v>1863.37</v>
-      </c>
-      <c r="G238" s="1">
         <v>488.38</v>
       </c>
-      <c r="H238" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I238" s="1">
+      <c r="G238">
+        <v>1358.31</v>
+      </c>
+      <c r="H238">
+        <v>588.4</v>
+      </c>
+      <c r="I238">
+        <v>0</v>
+      </c>
+      <c r="J238">
+        <v>0</v>
+      </c>
+      <c r="K238" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L238" s="1">
         <v>201.67</v>
       </c>
-      <c r="J238">
-        <v>0</v>
-      </c>
-      <c r="K238">
-        <v>0</v>
-      </c>
-      <c r="L238">
-        <v>1358.31</v>
-      </c>
       <c r="M238">
-        <v>588.4</v>
-      </c>
-      <c r="N238">
-        <v>0</v>
-      </c>
-      <c r="O238">
         <v>400</v>
       </c>
     </row>
-    <row r="239" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="239" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B239">
         <v>3144437</v>
       </c>
@@ -9331,41 +9171,35 @@
       <c r="D239">
         <v>0</v>
       </c>
-      <c r="E239">
-        <v>100</v>
+      <c r="E239" s="1">
+        <v>1855.44</v>
       </c>
       <c r="F239" s="1">
-        <v>1855.44</v>
-      </c>
-      <c r="G239" s="1">
         <v>484.58</v>
       </c>
-      <c r="H239" s="1" t="s">
+      <c r="G239">
+        <v>1363.41</v>
+      </c>
+      <c r="H239">
+        <v>588.4</v>
+      </c>
+      <c r="I239">
+        <v>0</v>
+      </c>
+      <c r="J239">
+        <v>0</v>
+      </c>
+      <c r="K239" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I239" s="1">
+      <c r="L239" s="1">
         <v>202.95</v>
       </c>
-      <c r="J239">
-        <v>0</v>
-      </c>
-      <c r="K239">
-        <v>0</v>
-      </c>
-      <c r="L239">
-        <v>1363.41</v>
-      </c>
       <c r="M239">
-        <v>588.4</v>
-      </c>
-      <c r="N239">
-        <v>0</v>
-      </c>
-      <c r="O239">
         <v>400</v>
       </c>
     </row>
-    <row r="240" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="240" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B240">
         <v>3144438</v>
       </c>
@@ -9375,41 +9209,35 @@
       <c r="D240">
         <v>0</v>
       </c>
-      <c r="E240">
-        <v>100</v>
+      <c r="E240" s="1">
+        <v>1847.51</v>
       </c>
       <c r="F240" s="1">
-        <v>1847.51</v>
-      </c>
-      <c r="G240" s="1">
         <v>481.38</v>
       </c>
-      <c r="H240" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I240" s="1">
+      <c r="G240">
+        <v>1368.51</v>
+      </c>
+      <c r="H240">
+        <v>588.4</v>
+      </c>
+      <c r="I240">
+        <v>0</v>
+      </c>
+      <c r="J240">
+        <v>0</v>
+      </c>
+      <c r="K240" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L240" s="1">
         <v>204.15</v>
       </c>
-      <c r="J240">
-        <v>0</v>
-      </c>
-      <c r="K240">
-        <v>0</v>
-      </c>
-      <c r="L240">
-        <v>1368.51</v>
-      </c>
       <c r="M240">
-        <v>588.4</v>
-      </c>
-      <c r="N240">
-        <v>0</v>
-      </c>
-      <c r="O240">
         <v>400</v>
       </c>
     </row>
-    <row r="241" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="241" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B241">
         <v>3144439</v>
       </c>
@@ -9419,41 +9247,35 @@
       <c r="D241">
         <v>0</v>
       </c>
-      <c r="E241">
-        <v>100</v>
+      <c r="E241" s="1">
+        <v>1839.57</v>
       </c>
       <c r="F241" s="1">
-        <v>1839.57</v>
-      </c>
-      <c r="G241" s="1">
         <v>478.78</v>
       </c>
-      <c r="H241" s="1" t="s">
+      <c r="G241">
+        <v>1373.61</v>
+      </c>
+      <c r="H241">
+        <v>588.4</v>
+      </c>
+      <c r="I241">
+        <v>0</v>
+      </c>
+      <c r="J241">
+        <v>0</v>
+      </c>
+      <c r="K241" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I241" s="1">
+      <c r="L241" s="1">
         <v>205.27</v>
       </c>
-      <c r="J241">
-        <v>0</v>
-      </c>
-      <c r="K241">
-        <v>0</v>
-      </c>
-      <c r="L241">
-        <v>1373.61</v>
-      </c>
       <c r="M241">
-        <v>588.4</v>
-      </c>
-      <c r="N241">
-        <v>0</v>
-      </c>
-      <c r="O241">
         <v>400</v>
       </c>
     </row>
-    <row r="242" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="242" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B242">
         <v>3144440</v>
       </c>
@@ -9463,41 +9285,35 @@
       <c r="D242">
         <v>0</v>
       </c>
-      <c r="E242">
-        <v>100</v>
+      <c r="E242" s="1">
+        <v>1831.64</v>
       </c>
       <c r="F242" s="1">
-        <v>1831.64</v>
-      </c>
-      <c r="G242" s="1">
         <v>476.78</v>
       </c>
-      <c r="H242" s="1" t="s">
+      <c r="G242">
+        <v>1378.71</v>
+      </c>
+      <c r="H242">
+        <v>588.4</v>
+      </c>
+      <c r="I242">
+        <v>0</v>
+      </c>
+      <c r="J242">
+        <v>0</v>
+      </c>
+      <c r="K242" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I242" s="1">
+      <c r="L242" s="1">
         <v>206.31</v>
       </c>
-      <c r="J242">
-        <v>0</v>
-      </c>
-      <c r="K242">
-        <v>0</v>
-      </c>
-      <c r="L242">
-        <v>1378.71</v>
-      </c>
       <c r="M242">
-        <v>588.4</v>
-      </c>
-      <c r="N242">
-        <v>0</v>
-      </c>
-      <c r="O242">
         <v>400</v>
       </c>
     </row>
-    <row r="243" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="243" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B243">
         <v>3144441</v>
       </c>
@@ -9507,41 +9323,35 @@
       <c r="D243">
         <v>0</v>
       </c>
-      <c r="E243">
-        <v>100</v>
+      <c r="E243" s="1">
+        <v>1823.71</v>
       </c>
       <c r="F243" s="1">
-        <v>1823.71</v>
-      </c>
-      <c r="G243" s="1">
         <v>475.38</v>
       </c>
-      <c r="H243" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I243" s="1">
+      <c r="G243">
+        <v>1383.81</v>
+      </c>
+      <c r="H243">
+        <v>588.4</v>
+      </c>
+      <c r="I243">
+        <v>0</v>
+      </c>
+      <c r="J243">
+        <v>0</v>
+      </c>
+      <c r="K243" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L243" s="1">
         <v>207.27</v>
       </c>
-      <c r="J243">
-        <v>0</v>
-      </c>
-      <c r="K243">
-        <v>0</v>
-      </c>
-      <c r="L243">
-        <v>1383.81</v>
-      </c>
       <c r="M243">
-        <v>588.4</v>
-      </c>
-      <c r="N243">
-        <v>0</v>
-      </c>
-      <c r="O243">
         <v>400</v>
       </c>
     </row>
-    <row r="244" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="244" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B244">
         <v>3144442</v>
       </c>
@@ -9551,41 +9361,35 @@
       <c r="D244">
         <v>0</v>
       </c>
-      <c r="E244">
-        <v>100</v>
+      <c r="E244" s="1">
+        <v>1815.77</v>
       </c>
       <c r="F244" s="1">
-        <v>1815.77</v>
-      </c>
-      <c r="G244" s="1">
         <v>474.58</v>
       </c>
-      <c r="H244" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I244" s="1">
+      <c r="G244">
+        <v>1388.91</v>
+      </c>
+      <c r="H244">
+        <v>588.4</v>
+      </c>
+      <c r="I244">
+        <v>0</v>
+      </c>
+      <c r="J244">
+        <v>0</v>
+      </c>
+      <c r="K244" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L244" s="1">
         <v>208.15</v>
       </c>
-      <c r="J244">
-        <v>0</v>
-      </c>
-      <c r="K244">
-        <v>0</v>
-      </c>
-      <c r="L244">
-        <v>1388.91</v>
-      </c>
       <c r="M244">
-        <v>588.4</v>
-      </c>
-      <c r="N244">
-        <v>0</v>
-      </c>
-      <c r="O244">
         <v>400</v>
       </c>
     </row>
-    <row r="245" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="245" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B245">
         <v>3144443</v>
       </c>
@@ -9595,41 +9399,35 @@
       <c r="D245">
         <v>0</v>
       </c>
-      <c r="E245">
-        <v>100</v>
+      <c r="E245" s="1">
+        <v>1807.84</v>
       </c>
       <c r="F245" s="1">
-        <v>1807.84</v>
-      </c>
-      <c r="G245" s="1">
         <v>474.38</v>
       </c>
-      <c r="H245" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I245" s="1">
+      <c r="G245">
+        <v>1394.01</v>
+      </c>
+      <c r="H245">
+        <v>588.4</v>
+      </c>
+      <c r="I245">
+        <v>0</v>
+      </c>
+      <c r="J245">
+        <v>0</v>
+      </c>
+      <c r="K245" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L245" s="1">
         <v>208.94</v>
       </c>
-      <c r="J245">
-        <v>0</v>
-      </c>
-      <c r="K245">
-        <v>0</v>
-      </c>
-      <c r="L245">
-        <v>1394.01</v>
-      </c>
       <c r="M245">
-        <v>588.4</v>
-      </c>
-      <c r="N245">
-        <v>0</v>
-      </c>
-      <c r="O245">
         <v>400</v>
       </c>
     </row>
-    <row r="246" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="246" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B246">
         <v>3144444</v>
       </c>
@@ -9639,41 +9437,35 @@
       <c r="D246">
         <v>0</v>
       </c>
-      <c r="E246">
-        <v>100</v>
+      <c r="E246" s="1">
+        <v>1799.91</v>
       </c>
       <c r="F246" s="1">
-        <v>1799.91</v>
-      </c>
-      <c r="G246" s="1">
         <v>474.78</v>
       </c>
-      <c r="H246" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I246" s="1">
+      <c r="G246">
+        <v>1399.11</v>
+      </c>
+      <c r="H246">
+        <v>588.4</v>
+      </c>
+      <c r="I246">
+        <v>0</v>
+      </c>
+      <c r="J246">
+        <v>0</v>
+      </c>
+      <c r="K246" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L246" s="1">
         <v>209.63</v>
       </c>
-      <c r="J246">
-        <v>0</v>
-      </c>
-      <c r="K246">
-        <v>0</v>
-      </c>
-      <c r="L246">
-        <v>1399.11</v>
-      </c>
       <c r="M246">
-        <v>588.4</v>
-      </c>
-      <c r="N246">
-        <v>0</v>
-      </c>
-      <c r="O246">
         <v>400</v>
       </c>
     </row>
-    <row r="247" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="247" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B247">
         <v>3144445</v>
       </c>
@@ -9683,41 +9475,35 @@
       <c r="D247">
         <v>0</v>
       </c>
-      <c r="E247">
-        <v>100</v>
+      <c r="E247" s="1">
+        <v>1791.97</v>
       </c>
       <c r="F247" s="1">
-        <v>1791.97</v>
-      </c>
-      <c r="G247" s="1">
         <v>475.78</v>
       </c>
-      <c r="H247" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I247" s="1">
+      <c r="G247">
+        <v>1404.21</v>
+      </c>
+      <c r="H247">
+        <v>588.4</v>
+      </c>
+      <c r="I247">
+        <v>0</v>
+      </c>
+      <c r="J247">
+        <v>0</v>
+      </c>
+      <c r="K247" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L247" s="1">
         <v>210.23</v>
       </c>
-      <c r="J247">
-        <v>0</v>
-      </c>
-      <c r="K247">
-        <v>0</v>
-      </c>
-      <c r="L247">
-        <v>1404.21</v>
-      </c>
       <c r="M247">
-        <v>588.4</v>
-      </c>
-      <c r="N247">
-        <v>0</v>
-      </c>
-      <c r="O247">
         <v>400</v>
       </c>
     </row>
-    <row r="248" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="248" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B248">
         <v>3144446</v>
       </c>
@@ -9727,41 +9513,35 @@
       <c r="D248">
         <v>0</v>
       </c>
-      <c r="E248">
-        <v>100</v>
+      <c r="E248" s="1">
+        <v>1784.04</v>
       </c>
       <c r="F248" s="1">
-        <v>1784.04</v>
-      </c>
-      <c r="G248" s="1">
         <v>477.38</v>
       </c>
-      <c r="H248" s="1" t="s">
+      <c r="G248">
+        <v>1409.31</v>
+      </c>
+      <c r="H248">
+        <v>588.4</v>
+      </c>
+      <c r="I248">
+        <v>0</v>
+      </c>
+      <c r="J248">
+        <v>0</v>
+      </c>
+      <c r="K248" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I248" s="1">
+      <c r="L248" s="1">
         <v>210.73</v>
       </c>
-      <c r="J248">
-        <v>0</v>
-      </c>
-      <c r="K248">
-        <v>0</v>
-      </c>
-      <c r="L248">
-        <v>1409.31</v>
-      </c>
       <c r="M248">
-        <v>588.4</v>
-      </c>
-      <c r="N248">
-        <v>0</v>
-      </c>
-      <c r="O248">
         <v>400</v>
       </c>
     </row>
-    <row r="249" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="249" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B249">
         <v>3144447</v>
       </c>
@@ -9771,41 +9551,35 @@
       <c r="D249">
         <v>0</v>
       </c>
-      <c r="E249">
-        <v>100</v>
+      <c r="E249" s="1">
+        <v>1776.11</v>
       </c>
       <c r="F249" s="1">
-        <v>1776.11</v>
-      </c>
-      <c r="G249" s="1">
         <v>479.58</v>
       </c>
-      <c r="H249" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I249" s="1">
+      <c r="G249">
+        <v>1414.41</v>
+      </c>
+      <c r="H249">
+        <v>588.4</v>
+      </c>
+      <c r="I249">
+        <v>0</v>
+      </c>
+      <c r="J249">
+        <v>0</v>
+      </c>
+      <c r="K249" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L249" s="1">
         <v>211.12</v>
       </c>
-      <c r="J249">
-        <v>0</v>
-      </c>
-      <c r="K249">
-        <v>0</v>
-      </c>
-      <c r="L249">
-        <v>1414.41</v>
-      </c>
       <c r="M249">
-        <v>588.4</v>
-      </c>
-      <c r="N249">
-        <v>0</v>
-      </c>
-      <c r="O249">
         <v>400</v>
       </c>
     </row>
-    <row r="250" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="250" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B250">
         <v>3144448</v>
       </c>
@@ -9815,41 +9589,35 @@
       <c r="D250">
         <v>0</v>
       </c>
-      <c r="E250">
-        <v>100</v>
+      <c r="E250" s="1">
+        <v>1768.17</v>
       </c>
       <c r="F250" s="1">
-        <v>1768.17</v>
-      </c>
-      <c r="G250" s="1">
         <v>482.38</v>
       </c>
-      <c r="H250" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I250" s="1">
+      <c r="G250">
+        <v>1418.85</v>
+      </c>
+      <c r="H250">
+        <v>588.4</v>
+      </c>
+      <c r="I250">
+        <v>0</v>
+      </c>
+      <c r="J250">
+        <v>0</v>
+      </c>
+      <c r="K250" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L250" s="1">
         <v>209.65</v>
       </c>
-      <c r="J250">
-        <v>0</v>
-      </c>
-      <c r="K250">
-        <v>0</v>
-      </c>
-      <c r="L250">
-        <v>1418.85</v>
-      </c>
       <c r="M250">
-        <v>588.4</v>
-      </c>
-      <c r="N250">
-        <v>0</v>
-      </c>
-      <c r="O250">
         <v>400</v>
       </c>
     </row>
-    <row r="251" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="251" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B251">
         <v>3144449</v>
       </c>
@@ -9859,41 +9627,35 @@
       <c r="D251">
         <v>0</v>
       </c>
-      <c r="E251">
-        <v>100</v>
+      <c r="E251" s="1">
+        <v>1760.24</v>
       </c>
       <c r="F251" s="1">
-        <v>1760.24</v>
-      </c>
-      <c r="G251" s="1">
         <v>485.78</v>
       </c>
-      <c r="H251" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I251" s="1">
+      <c r="G251">
+        <v>1423.37</v>
+      </c>
+      <c r="H251">
+        <v>588.4</v>
+      </c>
+      <c r="I251">
+        <v>0</v>
+      </c>
+      <c r="J251">
+        <v>0</v>
+      </c>
+      <c r="K251" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L251" s="1">
         <v>209.96</v>
       </c>
-      <c r="J251">
-        <v>0</v>
-      </c>
-      <c r="K251">
-        <v>0</v>
-      </c>
-      <c r="L251">
-        <v>1423.37</v>
-      </c>
       <c r="M251">
-        <v>588.4</v>
-      </c>
-      <c r="N251">
-        <v>0</v>
-      </c>
-      <c r="O251">
         <v>400</v>
       </c>
     </row>
-    <row r="252" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="252" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B252">
         <v>3144450</v>
       </c>
@@ -9903,41 +9665,35 @@
       <c r="D252">
         <v>0</v>
       </c>
-      <c r="E252">
-        <v>100</v>
+      <c r="E252" s="1">
+        <v>1752.31</v>
       </c>
       <c r="F252" s="1">
-        <v>1752.31</v>
-      </c>
-      <c r="G252" s="1">
         <v>489.78</v>
       </c>
-      <c r="H252" s="1" t="s">
+      <c r="G252">
+        <v>1427.97</v>
+      </c>
+      <c r="H252">
+        <v>588.4</v>
+      </c>
+      <c r="I252">
+        <v>0</v>
+      </c>
+      <c r="J252">
+        <v>1</v>
+      </c>
+      <c r="K252" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I252" s="1">
+      <c r="L252" s="1">
         <v>210.11</v>
       </c>
-      <c r="J252">
-        <v>1</v>
-      </c>
-      <c r="K252">
-        <v>0</v>
-      </c>
-      <c r="L252">
-        <v>1427.97</v>
-      </c>
       <c r="M252">
-        <v>588.4</v>
-      </c>
-      <c r="N252">
-        <v>0</v>
-      </c>
-      <c r="O252">
         <v>400</v>
       </c>
     </row>
-    <row r="253" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="253" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B253">
         <v>3144451</v>
       </c>
@@ -9947,41 +9703,35 @@
       <c r="D253">
         <v>0</v>
       </c>
-      <c r="E253">
-        <v>100</v>
+      <c r="E253" s="1">
+        <v>1739.41</v>
       </c>
       <c r="F253" s="1">
-        <v>1739.41</v>
-      </c>
-      <c r="G253" s="1">
         <v>499.58</v>
       </c>
-      <c r="H253" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I253" s="1">
+      <c r="G253">
+        <v>1433.53</v>
+      </c>
+      <c r="H253">
+        <v>588.4</v>
+      </c>
+      <c r="I253">
+        <v>0</v>
+      </c>
+      <c r="J253">
+        <v>1</v>
+      </c>
+      <c r="K253" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L253" s="1">
         <v>200.95</v>
       </c>
-      <c r="J253">
-        <v>1</v>
-      </c>
-      <c r="K253">
-        <v>0</v>
-      </c>
-      <c r="L253">
-        <v>1433.53</v>
-      </c>
       <c r="M253">
-        <v>588.4</v>
-      </c>
-      <c r="N253">
-        <v>0</v>
-      </c>
-      <c r="O253">
         <v>400</v>
       </c>
     </row>
-    <row r="254" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="254" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B254">
         <v>3144452</v>
       </c>
@@ -9991,41 +9741,35 @@
       <c r="D254">
         <v>0</v>
       </c>
-      <c r="E254">
-        <v>100</v>
+      <c r="E254" s="1">
+        <v>1734.19</v>
       </c>
       <c r="F254" s="1">
-        <v>1734.19</v>
-      </c>
-      <c r="G254" s="1">
         <v>505.38</v>
       </c>
-      <c r="H254" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I254" s="1">
+      <c r="G254">
+        <v>1434.81</v>
+      </c>
+      <c r="H254">
+        <v>588.4</v>
+      </c>
+      <c r="I254">
+        <v>0</v>
+      </c>
+      <c r="J254">
+        <v>1</v>
+      </c>
+      <c r="K254" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L254" s="1">
         <v>197.89</v>
       </c>
-      <c r="J254">
-        <v>1</v>
-      </c>
-      <c r="K254">
-        <v>0</v>
-      </c>
-      <c r="L254">
-        <v>1434.81</v>
-      </c>
       <c r="M254">
-        <v>588.4</v>
-      </c>
-      <c r="N254">
-        <v>0</v>
-      </c>
-      <c r="O254">
         <v>400</v>
       </c>
     </row>
-    <row r="255" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="255" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B255">
         <v>3144453</v>
       </c>
@@ -10035,41 +9779,35 @@
       <c r="D255">
         <v>0</v>
       </c>
-      <c r="E255">
-        <v>100</v>
+      <c r="E255" s="1">
+        <v>1729.66</v>
       </c>
       <c r="F255" s="1">
-        <v>1729.66</v>
-      </c>
-      <c r="G255" s="1">
         <v>511.78</v>
       </c>
-      <c r="H255" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I255" s="1">
+      <c r="G255">
+        <v>1435.25</v>
+      </c>
+      <c r="H255">
+        <v>588.4</v>
+      </c>
+      <c r="I255">
+        <v>0</v>
+      </c>
+      <c r="J255">
+        <v>1</v>
+      </c>
+      <c r="K255" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L255" s="1">
         <v>195.32</v>
       </c>
-      <c r="J255">
-        <v>1</v>
-      </c>
-      <c r="K255">
-        <v>0</v>
-      </c>
-      <c r="L255">
-        <v>1435.25</v>
-      </c>
       <c r="M255">
-        <v>588.4</v>
-      </c>
-      <c r="N255">
-        <v>0</v>
-      </c>
-      <c r="O255">
         <v>400</v>
       </c>
     </row>
-    <row r="256" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="256" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B256">
         <v>3144454</v>
       </c>
@@ -10079,41 +9817,35 @@
       <c r="D256">
         <v>0</v>
       </c>
-      <c r="E256">
-        <v>100</v>
+      <c r="E256" s="1">
+        <v>1725.71</v>
       </c>
       <c r="F256" s="1">
-        <v>1725.71</v>
-      </c>
-      <c r="G256" s="1">
         <v>518.78</v>
       </c>
-      <c r="H256" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I256" s="1">
+      <c r="G256">
+        <v>1434.97</v>
+      </c>
+      <c r="H256">
+        <v>588.4</v>
+      </c>
+      <c r="I256">
+        <v>0</v>
+      </c>
+      <c r="J256">
+        <v>1</v>
+      </c>
+      <c r="K256" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L256" s="1">
         <v>193.07</v>
       </c>
-      <c r="J256">
-        <v>1</v>
-      </c>
-      <c r="K256">
-        <v>0</v>
-      </c>
-      <c r="L256">
-        <v>1434.97</v>
-      </c>
       <c r="M256">
-        <v>588.4</v>
-      </c>
-      <c r="N256">
-        <v>0</v>
-      </c>
-      <c r="O256">
         <v>400</v>
       </c>
     </row>
-    <row r="257" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="257" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B257">
         <v>3144455</v>
       </c>
@@ -10123,41 +9855,35 @@
       <c r="D257">
         <v>0</v>
       </c>
-      <c r="E257">
-        <v>100</v>
+      <c r="E257" s="1">
+        <v>1722.28</v>
       </c>
       <c r="F257" s="1">
-        <v>1722.28</v>
-      </c>
-      <c r="G257" s="1">
         <v>526.38</v>
       </c>
-      <c r="H257" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I257" s="1">
+      <c r="G257">
+        <v>1434.07</v>
+      </c>
+      <c r="H257">
+        <v>588.4</v>
+      </c>
+      <c r="I257">
+        <v>0</v>
+      </c>
+      <c r="J257">
+        <v>1</v>
+      </c>
+      <c r="K257" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L257" s="1">
         <v>191.02</v>
       </c>
-      <c r="J257">
-        <v>1</v>
-      </c>
-      <c r="K257">
-        <v>0</v>
-      </c>
-      <c r="L257">
-        <v>1434.07</v>
-      </c>
       <c r="M257">
-        <v>588.4</v>
-      </c>
-      <c r="N257">
-        <v>0</v>
-      </c>
-      <c r="O257">
         <v>400</v>
       </c>
     </row>
-    <row r="258" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="258" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B258">
         <v>3144456</v>
       </c>
@@ -10167,41 +9893,35 @@
       <c r="D258">
         <v>0</v>
       </c>
-      <c r="E258">
-        <v>100</v>
+      <c r="E258" s="1">
+        <v>1719.3</v>
       </c>
       <c r="F258" s="1">
-        <v>1719.3</v>
-      </c>
-      <c r="G258" s="1">
         <v>534.58000000000004</v>
       </c>
-      <c r="H258" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I258" s="1">
+      <c r="G258">
+        <v>1432.61</v>
+      </c>
+      <c r="H258">
+        <v>588.4</v>
+      </c>
+      <c r="I258">
+        <v>0</v>
+      </c>
+      <c r="J258">
+        <v>1</v>
+      </c>
+      <c r="K258" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L258" s="1">
         <v>189.12</v>
       </c>
-      <c r="J258">
-        <v>1</v>
-      </c>
-      <c r="K258">
-        <v>0</v>
-      </c>
-      <c r="L258">
-        <v>1432.61</v>
-      </c>
       <c r="M258">
-        <v>588.4</v>
-      </c>
-      <c r="N258">
-        <v>0</v>
-      </c>
-      <c r="O258">
         <v>400</v>
       </c>
     </row>
-    <row r="259" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="259" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B259">
         <v>3144457</v>
       </c>
@@ -10211,41 +9931,35 @@
       <c r="D259">
         <v>0</v>
       </c>
-      <c r="E259">
-        <v>100</v>
+      <c r="E259" s="1">
+        <v>1716.71</v>
       </c>
       <c r="F259" s="1">
-        <v>1716.71</v>
-      </c>
-      <c r="G259" s="1">
         <v>543.38</v>
       </c>
-      <c r="H259" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I259" s="1">
+      <c r="G259">
+        <v>1430.68</v>
+      </c>
+      <c r="H259">
+        <v>588.4</v>
+      </c>
+      <c r="I259">
+        <v>0</v>
+      </c>
+      <c r="J259">
+        <v>1</v>
+      </c>
+      <c r="K259" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L259" s="1">
         <v>187.31</v>
       </c>
-      <c r="J259">
-        <v>1</v>
-      </c>
-      <c r="K259">
-        <v>0</v>
-      </c>
-      <c r="L259">
-        <v>1430.68</v>
-      </c>
       <c r="M259">
-        <v>588.4</v>
-      </c>
-      <c r="N259">
-        <v>0</v>
-      </c>
-      <c r="O259">
         <v>400</v>
       </c>
     </row>
-    <row r="260" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="260" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B260">
         <v>3144458</v>
       </c>
@@ -10255,41 +9969,35 @@
       <c r="D260">
         <v>0</v>
       </c>
-      <c r="E260">
-        <v>100</v>
+      <c r="E260" s="1">
+        <v>1714.61</v>
       </c>
       <c r="F260" s="1">
-        <v>1714.61</v>
-      </c>
-      <c r="G260" s="1">
         <v>552.13</v>
       </c>
-      <c r="H260" s="1" t="s">
+      <c r="G260">
+        <v>1428.34</v>
+      </c>
+      <c r="H260">
+        <v>588.4</v>
+      </c>
+      <c r="I260">
+        <v>0</v>
+      </c>
+      <c r="J260">
+        <v>1</v>
+      </c>
+      <c r="K260" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I260" s="1">
+      <c r="L260" s="1">
         <v>185.66</v>
       </c>
-      <c r="J260">
-        <v>1</v>
-      </c>
-      <c r="K260">
-        <v>0</v>
-      </c>
-      <c r="L260">
-        <v>1428.34</v>
-      </c>
       <c r="M260">
-        <v>588.4</v>
-      </c>
-      <c r="N260">
-        <v>0</v>
-      </c>
-      <c r="O260">
         <v>400</v>
       </c>
     </row>
-    <row r="261" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="261" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B261">
         <v>3144459</v>
       </c>
@@ -10299,41 +10007,35 @@
       <c r="D261">
         <v>0</v>
       </c>
-      <c r="E261">
-        <v>100</v>
+      <c r="E261" s="1">
+        <v>1712.65</v>
       </c>
       <c r="F261" s="1">
-        <v>1712.65</v>
-      </c>
-      <c r="G261" s="1">
         <v>544.13</v>
       </c>
-      <c r="H261" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I261" s="1">
+      <c r="G261">
+        <v>1425.63</v>
+      </c>
+      <c r="H261">
+        <v>588.4</v>
+      </c>
+      <c r="I261">
+        <v>0</v>
+      </c>
+      <c r="J261">
+        <v>1</v>
+      </c>
+      <c r="K261" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L261" s="1">
         <v>186.64</v>
       </c>
-      <c r="J261">
-        <v>1</v>
-      </c>
-      <c r="K261">
-        <v>0</v>
-      </c>
-      <c r="L261">
-        <v>1425.63</v>
-      </c>
       <c r="M261">
-        <v>588.4</v>
-      </c>
-      <c r="N261">
-        <v>0</v>
-      </c>
-      <c r="O261">
         <v>400</v>
       </c>
     </row>
-    <row r="262" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="262" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B262">
         <v>3144460</v>
       </c>
@@ -10343,41 +10045,35 @@
       <c r="D262">
         <v>0</v>
       </c>
-      <c r="E262">
-        <v>100</v>
+      <c r="E262" s="1">
+        <v>1710.94</v>
       </c>
       <c r="F262" s="1">
-        <v>1710.94</v>
-      </c>
-      <c r="G262" s="1">
         <v>536.73</v>
       </c>
-      <c r="H262" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I262" s="1">
+      <c r="G262">
+        <v>1422.62</v>
+      </c>
+      <c r="H262">
+        <v>588.4</v>
+      </c>
+      <c r="I262">
+        <v>0</v>
+      </c>
+      <c r="J262">
+        <v>1</v>
+      </c>
+      <c r="K262" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L262" s="1">
         <v>187.48</v>
       </c>
-      <c r="J262">
-        <v>1</v>
-      </c>
-      <c r="K262">
-        <v>0</v>
-      </c>
-      <c r="L262">
-        <v>1422.62</v>
-      </c>
       <c r="M262">
-        <v>588.4</v>
-      </c>
-      <c r="N262">
-        <v>0</v>
-      </c>
-      <c r="O262">
         <v>400</v>
       </c>
     </row>
-    <row r="263" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="263" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B263">
         <v>3144461</v>
       </c>
@@ -10387,41 +10083,35 @@
       <c r="D263">
         <v>0</v>
       </c>
-      <c r="E263">
-        <v>100</v>
+      <c r="E263" s="1">
+        <v>1709.46</v>
       </c>
       <c r="F263" s="1">
-        <v>1709.46</v>
-      </c>
-      <c r="G263" s="1">
         <v>529.92999999999995</v>
       </c>
-      <c r="H263" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I263" s="1">
+      <c r="G263">
+        <v>1419.33</v>
+      </c>
+      <c r="H263">
+        <v>588.4</v>
+      </c>
+      <c r="I263">
+        <v>0</v>
+      </c>
+      <c r="J263">
+        <v>1</v>
+      </c>
+      <c r="K263" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L263" s="1">
         <v>188.19</v>
       </c>
-      <c r="J263">
-        <v>1</v>
-      </c>
-      <c r="K263">
-        <v>0</v>
-      </c>
-      <c r="L263">
-        <v>1419.33</v>
-      </c>
       <c r="M263">
-        <v>588.4</v>
-      </c>
-      <c r="N263">
-        <v>0</v>
-      </c>
-      <c r="O263">
         <v>400</v>
       </c>
     </row>
-    <row r="264" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="264" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B264">
         <v>3144462</v>
       </c>
@@ -10431,41 +10121,35 @@
       <c r="D264">
         <v>0</v>
       </c>
-      <c r="E264">
-        <v>100</v>
+      <c r="E264" s="1">
+        <v>1708.17</v>
       </c>
       <c r="F264" s="1">
-        <v>1708.17</v>
-      </c>
-      <c r="G264" s="1">
         <v>523.73</v>
       </c>
-      <c r="H264" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I264" s="1">
+      <c r="G264">
+        <v>1415.81</v>
+      </c>
+      <c r="H264">
+        <v>588.4</v>
+      </c>
+      <c r="I264">
+        <v>0</v>
+      </c>
+      <c r="J264">
+        <v>1</v>
+      </c>
+      <c r="K264" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L264" s="1">
         <v>188.79</v>
       </c>
-      <c r="J264">
-        <v>1</v>
-      </c>
-      <c r="K264">
-        <v>0</v>
-      </c>
-      <c r="L264">
-        <v>1415.81</v>
-      </c>
       <c r="M264">
-        <v>588.4</v>
-      </c>
-      <c r="N264">
-        <v>0</v>
-      </c>
-      <c r="O264">
         <v>400</v>
       </c>
     </row>
-    <row r="265" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="265" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B265">
         <v>3144463</v>
       </c>
@@ -10475,41 +10159,35 @@
       <c r="D265">
         <v>0</v>
       </c>
-      <c r="E265">
-        <v>100</v>
+      <c r="E265" s="1">
+        <v>1707.05</v>
       </c>
       <c r="F265" s="1">
-        <v>1707.05</v>
-      </c>
-      <c r="G265" s="1">
         <v>518.13</v>
       </c>
-      <c r="H265" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I265" s="1">
+      <c r="G265">
+        <v>1412.08</v>
+      </c>
+      <c r="H265">
+        <v>588.4</v>
+      </c>
+      <c r="I265">
+        <v>0</v>
+      </c>
+      <c r="J265">
+        <v>1</v>
+      </c>
+      <c r="K265" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L265" s="1">
         <v>189.28</v>
       </c>
-      <c r="J265">
-        <v>1</v>
-      </c>
-      <c r="K265">
-        <v>0</v>
-      </c>
-      <c r="L265">
-        <v>1412.08</v>
-      </c>
       <c r="M265">
-        <v>588.4</v>
-      </c>
-      <c r="N265">
-        <v>0</v>
-      </c>
-      <c r="O265">
         <v>400</v>
       </c>
     </row>
-    <row r="266" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="266" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B266">
         <v>3144464</v>
       </c>
@@ -10519,41 +10197,35 @@
       <c r="D266">
         <v>0</v>
       </c>
-      <c r="E266">
-        <v>100</v>
+      <c r="E266" s="1">
+        <v>1706.07</v>
       </c>
       <c r="F266" s="1">
-        <v>1706.07</v>
-      </c>
-      <c r="G266" s="1">
         <v>513.13</v>
       </c>
-      <c r="H266" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I266" s="1">
+      <c r="G266">
+        <v>1408.17</v>
+      </c>
+      <c r="H266">
+        <v>588.4</v>
+      </c>
+      <c r="I266">
+        <v>0</v>
+      </c>
+      <c r="J266">
+        <v>1</v>
+      </c>
+      <c r="K266" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L266" s="1">
         <v>189.68</v>
       </c>
-      <c r="J266">
-        <v>1</v>
-      </c>
-      <c r="K266">
-        <v>0</v>
-      </c>
-      <c r="L266">
-        <v>1408.17</v>
-      </c>
       <c r="M266">
-        <v>588.4</v>
-      </c>
-      <c r="N266">
-        <v>0</v>
-      </c>
-      <c r="O266">
         <v>400</v>
       </c>
     </row>
-    <row r="267" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="267" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B267">
         <v>3144465</v>
       </c>
@@ -10563,37 +10235,31 @@
       <c r="D267">
         <v>0</v>
       </c>
-      <c r="E267">
-        <v>100</v>
+      <c r="E267" s="1">
+        <v>1705.22</v>
       </c>
       <c r="F267" s="1">
-        <v>1705.22</v>
-      </c>
-      <c r="G267" s="1">
         <v>508.73</v>
       </c>
-      <c r="H267" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I267" s="1">
+      <c r="G267">
+        <v>1404.11</v>
+      </c>
+      <c r="H267">
+        <v>588.4</v>
+      </c>
+      <c r="I267">
+        <v>0</v>
+      </c>
+      <c r="J267">
+        <v>1</v>
+      </c>
+      <c r="K267" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L267" s="1">
         <v>189.99</v>
       </c>
-      <c r="J267">
-        <v>1</v>
-      </c>
-      <c r="K267">
-        <v>0</v>
-      </c>
-      <c r="L267">
-        <v>1404.11</v>
-      </c>
       <c r="M267">
-        <v>588.4</v>
-      </c>
-      <c r="N267">
-        <v>0</v>
-      </c>
-      <c r="O267">
         <v>400</v>
       </c>
     </row>

</xml_diff>